<commit_message>
feat: Implemented System Login
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nbg\Desktop\UIPath Professional Developer\ACME_ClientSecurityHash_REF\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FAA57E0-8117-45E9-AF20-F2FF32B6F8C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{603355E7-6DAE-4D05-B140-40050AC2AE1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="55">
   <si>
     <t>Name</t>
   </si>
@@ -175,10 +175,19 @@
     <t>exceptions@acme-test.com</t>
   </si>
   <si>
-    <t>System1Credential</t>
-  </si>
-  <si>
     <t>ACME_Credential</t>
+  </si>
+  <si>
+    <t>ACME_Automation</t>
+  </si>
+  <si>
+    <t>Folder name. The value must match a folder defined in Orchestrator. For classic folders leave the value field empty.</t>
+  </si>
+  <si>
+    <t>OrchestratorFolder</t>
+  </si>
+  <si>
+    <t>System1_Credential</t>
   </si>
 </sst>
 </file>
@@ -565,14 +574,14 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="43.5703125" customWidth="1"/>
     <col min="2" max="2" width="47.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="81.42578125" customWidth="1"/>
+    <col min="3" max="3" width="180.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -648,37 +657,42 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" t="s">
-        <v>46</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>47</v>
+        <v>54</v>
+      </c>
+      <c r="B10" t="s">
+        <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
-        <v>50</v>
-      </c>
-      <c r="B14" t="s">
-        <v>51</v>
+        <v>48</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" ht="14.25" customHeight="1"/>
-    <row r="18" ht="14.25" customHeight="1"/>
+    <row r="16" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A16" t="s">
+        <v>53</v>
+      </c>
+      <c r="B16" t="s">
+        <v>51</v>
+      </c>
+      <c r="C16" t="s">
+        <v>52</v>
+      </c>
+    </row>
     <row r="19" ht="14.25" customHeight="1"/>
     <row r="20" ht="14.25" customHeight="1"/>
     <row r="21" ht="14.25" customHeight="1"/>
@@ -1662,8 +1676,8 @@
   </sheetData>
   <phoneticPr fontId="2"/>
   <hyperlinks>
-    <hyperlink ref="B12" r:id="rId1" xr:uid="{95AE6EBD-DB68-45BD-A43F-7C46CF2639D0}"/>
-    <hyperlink ref="B10" r:id="rId2" xr:uid="{E83B0CED-EC86-4D77-81D4-3E76E9D638A5}"/>
+    <hyperlink ref="B14" r:id="rId1" xr:uid="{95AE6EBD-DB68-45BD-A43F-7C46CF2639D0}"/>
+    <hyperlink ref="B12" r:id="rId2" xr:uid="{E83B0CED-EC86-4D77-81D4-3E76E9D638A5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>

</xml_diff>

<commit_message>
chore: updated arguments for inputs
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nbg\Desktop\UIPath Professional Developer\ACME_ClientSecurityHash_REF\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{603355E7-6DAE-4D05-B140-40050AC2AE1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83ED54B8-9E54-49B0-BF02-44390B3E4611}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -148,9 +148,6 @@
     <t>System1_URL</t>
   </si>
   <si>
-    <t>https://acme-test.uipath.com/login</t>
-  </si>
-  <si>
     <t>System1_WorkItemsURL</t>
   </si>
   <si>
@@ -188,6 +185,9 @@
   </si>
   <si>
     <t>System1_Credential</t>
+  </si>
+  <si>
+    <t>https://acme-test.uipath.com/</t>
   </si>
 </sst>
 </file>
@@ -574,7 +574,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -635,62 +635,62 @@
       <c r="A4" t="s">
         <v>40</v>
       </c>
-      <c r="B4" t="s">
-        <v>41</v>
+      <c r="B4" s="4" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:26"/>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" t="s">
         <v>42</v>
-      </c>
-      <c r="B6" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" t="s">
         <v>44</v>
-      </c>
-      <c r="B8" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12" s="4" t="s">
         <v>46</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
+        <v>47</v>
+      </c>
+      <c r="B14" s="4" t="s">
         <v>48</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="A16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B16" t="s">
+        <v>50</v>
+      </c>
+      <c r="C16" t="s">
         <v>51</v>
-      </c>
-      <c r="C16" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="19" ht="14.25" customHeight="1"/>
@@ -1678,9 +1678,10 @@
   <hyperlinks>
     <hyperlink ref="B14" r:id="rId1" xr:uid="{95AE6EBD-DB68-45BD-A43F-7C46CF2639D0}"/>
     <hyperlink ref="B12" r:id="rId2" xr:uid="{E83B0CED-EC86-4D77-81D4-3E76E9D638A5}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{FCE1AA14-8DE0-4F33-BD35-E835329EE20C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
feat: added exception handling
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nbg\Desktop\UIPath Professional Developer\ACME_ClientSecurityHash_REF\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83ED54B8-9E54-49B0-BF02-44390B3E4611}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3614258-5316-4D9F-A02E-9AFD779ABC4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -157,9 +157,6 @@
     <t>System1_UpdateWorkItemURL</t>
   </si>
   <si>
-    <t>https://acme-test.uipath.com/work-items/update/</t>
-  </si>
-  <si>
     <t>SHA1_URL</t>
   </si>
   <si>
@@ -188,6 +185,9 @@
   </si>
   <si>
     <t>https://acme-test.uipath.com/</t>
+  </si>
+  <si>
+    <t>https://acme-test.uipath.com/work-items/update</t>
   </si>
 </sst>
 </file>
@@ -574,7 +574,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -636,7 +636,7 @@
         <v>40</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:26"/>
@@ -653,44 +653,44 @@
       <c r="A8" t="s">
         <v>43</v>
       </c>
-      <c r="B8" t="s">
-        <v>44</v>
+      <c r="B8" s="4" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
+        <v>44</v>
+      </c>
+      <c r="B12" s="4" t="s">
         <v>45</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
+        <v>46</v>
+      </c>
+      <c r="B14" s="4" t="s">
         <v>47</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="A16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B16" t="s">
+        <v>49</v>
+      </c>
+      <c r="C16" t="s">
         <v>50</v>
-      </c>
-      <c r="C16" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="19" ht="14.25" customHeight="1"/>
@@ -1679,9 +1679,10 @@
     <hyperlink ref="B14" r:id="rId1" xr:uid="{95AE6EBD-DB68-45BD-A43F-7C46CF2639D0}"/>
     <hyperlink ref="B12" r:id="rId2" xr:uid="{E83B0CED-EC86-4D77-81D4-3E76E9D638A5}"/>
     <hyperlink ref="B4" r:id="rId3" xr:uid="{FCE1AA14-8DE0-4F33-BD35-E835329EE20C}"/>
+    <hyperlink ref="B8" r:id="rId4" xr:uid="{4856C092-3C74-4078-9E11-C8E262BE1260}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
 

</xml_diff>